<commit_message>
Creating a common DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -48,6 +49,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Raman Arora</t>
+  </si>
+  <si>
+    <t>Rupee</t>
   </si>
 </sst>
 </file>
@@ -368,7 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -409,4 +422,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Parameterization and automating the third test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8175" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>firstname</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Rupee</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Ishita</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Sehgal</t>
   </si>
 </sst>
 </file>
@@ -379,15 +391,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -415,6 +428,48 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -428,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Setting up run modes for Test data and implementing parameterization
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ОБУЧЕНИЕ\Automation Architect - Selenium WebDriver - 7 Live Projects\eclipse\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>firstname</t>
   </si>
@@ -95,19 +95,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>runmode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -135,7 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -151,9 +153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,14 +193,14 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -231,9 +233,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -263,7 +265,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -415,14 +417,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -453,30 +452,25 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +483,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -503,8 +500,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -517,8 +517,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -531,8 +534,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -545,10 +551,12 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -557,7 +565,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>